<commit_message>
ENVOI DES FONCTIONS POUR PUBLIER
</commit_message>
<xml_diff>
--- a/doc/MODEL IMPORTATION ODOO.xlsx
+++ b/doc/MODEL IMPORTATION ODOO.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJET\M_H_INTERFACE\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,117 +26,113 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
-    <t xml:space="preserve">ncc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom d'affichage du partenaire de la facture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Produit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Prix unitaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Quantité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Unité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lignes de facture/Remise (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montant hors taxes signé dans la devise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total signé en devises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statut en cours de paiement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1277774D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARROUCHE ABIDJAN SARL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00091 (S00119) [MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comptabilisé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00091 (S00119) [MC1001305] MILNET - Dégraissant super actif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MC1001305] MILNET - Dégraissant super actif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00091 (S00119) [MH1001105] HYGIMED - Détergent Désinfectant Bactéricide et fongicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MH1001105] HYGIMED - Détergent Désinfectant Bactéricide et fongicide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1444787X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Napizza Abidjan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00090 (S00118) [MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00090 (S00118) [MC1001305] MILNET - Dégraissant super actif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00090 (S00118) [MH3000505] MITAR X - Nettoyant Détartrant Sanitaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MH3000505] MITAR X - Nettoyant Détartrant Sanitaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">458844AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'AVENUE HOTEL APARTEMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV/2026/00089 (S00117) [MH3000405] MIDEO - Nettoyant Désinfectant sanitaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MH3000405] MIDEO - Nettoyant Désinfectant sanitaire</t>
+    <t>ncc</t>
+  </si>
+  <si>
+    <t>Nom d'affichage du partenaire de la facture</t>
+  </si>
+  <si>
+    <t>Lignes de facture</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Taxes</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Produit</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Prix unitaire</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Quantité</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Unité</t>
+  </si>
+  <si>
+    <t>Lignes de facture/Remise (%)</t>
+  </si>
+  <si>
+    <t>Montant hors taxes signé dans la devise</t>
+  </si>
+  <si>
+    <t>Taxe</t>
+  </si>
+  <si>
+    <t>Total signé en devises</t>
+  </si>
+  <si>
+    <t>Statut en cours de paiement</t>
+  </si>
+  <si>
+    <t>1277774D</t>
+  </si>
+  <si>
+    <t>MARROUCHE ABIDJAN SARL</t>
+  </si>
+  <si>
+    <t>INV/2026/00091 (S00119) [MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
+  </si>
+  <si>
+    <t>18%</t>
+  </si>
+  <si>
+    <t>[MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Comptabilisé</t>
+  </si>
+  <si>
+    <t>INV/2026/00091 (S00119) [MC1001305] MILNET - Dégraissant super actif</t>
+  </si>
+  <si>
+    <t>[MC1001305] MILNET - Dégraissant super actif</t>
+  </si>
+  <si>
+    <t>INV/2026/00091 (S00119) [MH1001105] HYGIMED - Détergent Désinfectant Bactéricide et fongicide</t>
+  </si>
+  <si>
+    <t>[MH1001105] HYGIMED - Détergent Désinfectant Bactéricide et fongicide</t>
+  </si>
+  <si>
+    <t>1444787X</t>
+  </si>
+  <si>
+    <t>Napizza Abidjan</t>
+  </si>
+  <si>
+    <t>INV/2026/00090 (S00118) [MH1000505] MIAFOUR - Rénovation fours, plaques et grils</t>
+  </si>
+  <si>
+    <t>INV/2026/00090 (S00118) [MC1001305] MILNET - Dégraissant super actif</t>
+  </si>
+  <si>
+    <t>INV/2026/00090 (S00118) [MH3000505] MITAR X - Nettoyant Détartrant Sanitaire</t>
+  </si>
+  <si>
+    <t>[MH3000505] MITAR X - Nettoyant Détartrant Sanitaire</t>
+  </si>
+  <si>
+    <t>458844AD</t>
+  </si>
+  <si>
+    <t>L'AVENUE HOTEL APARTEMENTS</t>
+  </si>
+  <si>
+    <t>INV/2026/00089 (S00117) [MH3000405] MIDEO - Nettoyant Désinfectant sanitaire</t>
+  </si>
+  <si>
+    <t>[MH3000405] MIDEO - Nettoyant Désinfectant sanitaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,22 +141,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,7 +158,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -181,100 +166,77 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -282,12 +244,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -316,7 +278,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -337,7 +299,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -388,7 +350,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -406,31 +368,32 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="30.71"/>
+    <col min="1" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="7" customWidth="1"/>
+    <col min="7" max="13" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +409,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -471,7 +434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -487,32 +450,32 @@
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="6">
         <v>3150</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="4">
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="n">
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
         <v>102600</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="4">
         <v>18468</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="4">
         <v>121068</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>20</v>
@@ -523,16 +486,16 @@
       <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="6">
         <v>3555</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="4">
         <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="4">
         <v>0</v>
       </c>
       <c r="J3" s="3"/>
@@ -540,7 +503,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>22</v>
@@ -551,16 +514,16 @@
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="6">
         <v>3555</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="4">
         <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="4">
         <v>0</v>
       </c>
       <c r="J4" s="3"/>
@@ -568,7 +531,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -584,32 +547,32 @@
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="6">
         <v>3150</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="4">
         <v>10</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="n">
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
         <v>121050</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="4">
         <v>21789</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="4">
         <v>142839</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>27</v>
@@ -620,16 +583,16 @@
       <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="6">
         <v>3555</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="4">
         <v>10</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="4">
         <v>0</v>
       </c>
       <c r="J6" s="3"/>
@@ -637,7 +600,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>28</v>
@@ -648,16 +611,16 @@
       <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="6">
         <v>2700</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="4">
         <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="4">
         <v>0</v>
       </c>
       <c r="J7" s="3"/>
@@ -665,7 +628,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -681,25 +644,25 @@
       <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="6">
         <v>2835</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="4">
         <v>30</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4" t="n">
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
         <v>85050</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="4">
         <v>15309</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" s="4">
         <v>100359</v>
       </c>
       <c r="M8" s="3" t="s">
@@ -707,12 +670,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>